<commit_message>
Desarrollo modulo predictivo trasnformaciones e hiperparametros, centralización de proyecto en estrutura API REST donde se han puesto a dispocisión de servicios de los modulos predictivo transformaciones e hiperparametros, pendiente de pasar servicios de los modulos disponibles al momento
</commit_message>
<xml_diff>
--- a/DiccionarioDatosUD.xlsx
+++ b/DiccionarioDatosUD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Documentos\INTEVO\U-Distrital\UNIVERSIDAD-DISTRITAL-PROYECTO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1F6E6D6-8A2F-4604-83EF-7407D3FA0B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E717C8-4C1A-4DA6-8228-D547D66B1B23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22125" yWindow="1200" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="563">
   <si>
     <t>GENERO</t>
   </si>
@@ -1654,6 +1654,66 @@
   </si>
   <si>
     <t>DESCRIPCION</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_UNO</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_DOS</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (1 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_TRES</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_CUATRO</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_CINCO</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_SEIS</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_SIETE</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_OCHO</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_NUEVE</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO_DIEZ</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (2 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (3 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (4 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (5 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (6 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (7 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (8 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (9 SEMESTRE)</t>
+  </si>
+  <si>
+    <t>RENDIMIENTO ESTUDIANTE (10 SEMESTRE)</t>
   </si>
 </sst>
 </file>
@@ -1683,7 +1743,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1706,17 +1766,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1725,7 +1774,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2006,10 +2055,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B349"/>
+  <dimension ref="A1:B358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
-      <selection activeCell="B353" sqref="B353"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="C360" sqref="C360"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4803,8 +4852,84 @@
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A349" s="3"/>
-      <c r="B349" s="3"/>
+      <c r="A349" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="B349" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A350" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="B350" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A351" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="B351" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A352" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="B352" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A353" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="B353" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A354" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="B354" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A355" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="B355" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A356" s="3" t="s">
+        <v>551</v>
+      </c>
+      <c r="B356" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A357" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="B357" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A358" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="B358" s="1" t="s">
+        <v>562</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>